<commit_message>
Added third measurement to analysis.
</commit_message>
<xml_diff>
--- a/tests/Analysis.xlsx
+++ b/tests/Analysis.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\edgetx\TX16S_HallDriftComp\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7032BC55-BBB5-4C53-ABB7-F75E1031D971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E6E2B9-31FB-4234-BD85-56F0BF9E1341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1 13°C" sheetId="1" r:id="rId1"/>
     <sheet name="Test2 18°C" sheetId="2" r:id="rId2"/>
-    <sheet name="Analogs" sheetId="4" r:id="rId3"/>
-    <sheet name="STM32 core temp" sheetId="3" r:id="rId4"/>
-    <sheet name="Low end abs" sheetId="5" r:id="rId5"/>
-    <sheet name="Low end rel" sheetId="6" r:id="rId6"/>
-    <sheet name="Mid abs" sheetId="7" r:id="rId7"/>
-    <sheet name="Mid rel" sheetId="8" r:id="rId8"/>
-    <sheet name="High end abs" sheetId="9" r:id="rId9"/>
-    <sheet name="High end rel" sheetId="10" r:id="rId10"/>
+    <sheet name="Test2 23°C" sheetId="11" r:id="rId3"/>
+    <sheet name="Analogs" sheetId="4" r:id="rId4"/>
+    <sheet name="STM32 core temp" sheetId="3" r:id="rId5"/>
+    <sheet name="Low end abs" sheetId="5" r:id="rId6"/>
+    <sheet name="Low end rel" sheetId="6" r:id="rId7"/>
+    <sheet name="Mid abs" sheetId="7" r:id="rId8"/>
+    <sheet name="Mid rel" sheetId="8" r:id="rId9"/>
+    <sheet name="High end abs" sheetId="9" r:id="rId10"/>
+    <sheet name="High end rel" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="14">
   <si>
     <t>Time [s]</t>
   </si>
@@ -1555,6 +1556,259 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Test2 23°C'!$A$4:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>2.2360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4580000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.532</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7539999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.827999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.901999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.976000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.124000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.271999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.346</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.494</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.568000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.641999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.716000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.79</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25.864000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26.937999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28.012</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29.085999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.16</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31.234000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32.308</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33.381999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34.456000000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35.53</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36.603999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37.677999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38.752000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Test2 23°C'!$B$4:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>26.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.63</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30.32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30.32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30.63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.32</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.63</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30.63</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>30.95</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3200-4EF0-83E8-8A5B496F0E2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1819,8 +2073,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.78585541351057353"/>
           <c:y val="0.71245480087437352"/>
-          <c:w val="8.7024657399992517E-2"/>
-          <c:h val="0.10197872901257249"/>
+          <c:w val="8.7074727967077881E-2"/>
+          <c:h val="0.15283200405409245"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2027,6 +2281,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2041,6 +2298,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2094,6 +2354,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2108,6 +2371,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>772</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2161,6 +2427,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2175,6 +2444,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,6 +2500,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2242,6 +2517,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2295,6 +2573,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2309,6 +2590,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,6 +2619,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2792,6 +3077,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2806,6 +3094,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2859,6 +3150,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2873,6 +3167,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2926,6 +3223,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2940,6 +3240,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2993,6 +3296,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3007,6 +3313,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3060,6 +3369,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3074,6 +3386,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3100,6 +3415,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3563,6 +3879,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3577,6 +3896,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3630,6 +3952,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3644,6 +3969,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3697,6 +4025,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3711,6 +4042,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3764,6 +4098,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3778,6 +4115,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3831,6 +4171,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3845,6 +4188,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3871,6 +4217,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4323,6 +4670,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4337,6 +4687,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4390,6 +4743,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4404,6 +4760,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4457,6 +4816,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4471,6 +4833,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4524,6 +4889,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4538,6 +4906,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4591,6 +4962,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4605,6 +4979,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4631,6 +5008,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5094,6 +5472,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5108,6 +5489,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3449</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5161,6 +5545,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5175,6 +5562,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5228,6 +5618,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5242,6 +5635,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5295,6 +5691,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5309,6 +5708,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3414</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5362,6 +5764,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5375,6 +5780,9 @@
                   <c:v>2619</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2623</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2623</c:v>
                 </c:pt>
               </c:numCache>
@@ -5402,6 +5810,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5854,6 +6263,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5868,6 +6280,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5921,6 +6336,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5935,6 +6353,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5988,6 +6409,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6002,6 +6426,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6055,6 +6482,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6069,6 +6499,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6122,6 +6555,9 @@
                 <c:pt idx="1">
                   <c:v>18.25</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6135,6 +6571,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -6162,6 +6601,7 @@
         <c:axId val="487041615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -10509,7 +10949,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -10542,7 +10982,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -10575,7 +11015,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -10608,7 +11048,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -10641,7 +11081,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -10674,7 +11114,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305604" cy="6009312"/>
+    <xdr:ext cx="9300253" cy="6014663"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -16956,8 +17396,2118 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC572C1-6D11-4774-B1B4-C1F25D80A2A5}">
+  <dimension ref="A1:R38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:R38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="8"/>
+    <col min="2" max="2" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="19"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2.2360000000000002</v>
+      </c>
+      <c r="B4" s="6">
+        <v>26.83</v>
+      </c>
+      <c r="C4" s="7">
+        <v>22.94</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2181</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2183</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2188</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3292</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3298</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3302</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2081</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2083</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2088</v>
+      </c>
+      <c r="M4" s="3">
+        <v>2106</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2109</v>
+      </c>
+      <c r="O4" s="4">
+        <v>2112</v>
+      </c>
+      <c r="P4" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R4" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3.31</v>
+      </c>
+      <c r="B5" s="6">
+        <v>27.78</v>
+      </c>
+      <c r="C5" s="7">
+        <v>22.94</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2180</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2183</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2188</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3292</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3296</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3302</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2081</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2106</v>
+      </c>
+      <c r="N5" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P5" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R5" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4.3840000000000003</v>
+      </c>
+      <c r="B6" s="6">
+        <v>27.78</v>
+      </c>
+      <c r="C6" s="7">
+        <v>22.94</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2179</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2181</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2188</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3292</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3298</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3303</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2105</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2109</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P6" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R6" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5.4580000000000002</v>
+      </c>
+      <c r="B7" s="6">
+        <v>28.41</v>
+      </c>
+      <c r="C7" s="7">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2179</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2189</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2189</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3292</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3295</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3303</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N7" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P7" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R7" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6.532</v>
+      </c>
+      <c r="B8" s="6">
+        <v>29.05</v>
+      </c>
+      <c r="C8" s="7">
+        <v>23.06</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2179</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2189</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3292</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3299</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3303</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2081</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N8" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P8" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R8" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7.6059999999999999</v>
+      </c>
+      <c r="B9" s="6">
+        <v>28.1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>23.06</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2179</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2184</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2252</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1222</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1222</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3306</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2082</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2110</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P9" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R9" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8.68</v>
+      </c>
+      <c r="B10" s="6">
+        <v>29.05</v>
+      </c>
+      <c r="C10" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2175</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2252</v>
+      </c>
+      <c r="G10" s="3">
+        <v>778</v>
+      </c>
+      <c r="H10" s="4">
+        <v>780</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3306</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N10" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P10" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R10" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9.7539999999999996</v>
+      </c>
+      <c r="B11" s="6">
+        <v>29.37</v>
+      </c>
+      <c r="C11" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2175</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2188</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2252</v>
+      </c>
+      <c r="G11" s="3">
+        <v>778</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3308</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3311</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2083</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M11" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2110</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P11" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R11" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10.827999999999999</v>
+      </c>
+      <c r="B12" s="6">
+        <v>29.37</v>
+      </c>
+      <c r="C12" s="7">
+        <v>23.06</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2175</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2252</v>
+      </c>
+      <c r="G12" s="3">
+        <v>778</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2558</v>
+      </c>
+      <c r="I12" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J12" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L12" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N12" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O12" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P12" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R12" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11.901999999999999</v>
+      </c>
+      <c r="B13" s="6">
+        <v>29.68</v>
+      </c>
+      <c r="C13" s="7">
+        <v>23.06</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2172</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2173</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2252</v>
+      </c>
+      <c r="G13" s="3">
+        <v>772</v>
+      </c>
+      <c r="H13" s="4">
+        <v>778</v>
+      </c>
+      <c r="I13" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N13" s="4">
+        <v>2110</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P13" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R13" s="7">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12.976000000000001</v>
+      </c>
+      <c r="B14" s="6">
+        <v>29.37</v>
+      </c>
+      <c r="C14" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2172</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3417</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3417</v>
+      </c>
+      <c r="G14" s="3">
+        <v>772</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2201</v>
+      </c>
+      <c r="I14" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J14" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2083</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M14" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N14" s="4">
+        <v>2112</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P14" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R14" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14.05</v>
+      </c>
+      <c r="B15" s="6">
+        <v>29.37</v>
+      </c>
+      <c r="C15" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2172</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3430</v>
+      </c>
+      <c r="F15" s="4">
+        <v>3432</v>
+      </c>
+      <c r="G15" s="3">
+        <v>772</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2182</v>
+      </c>
+      <c r="I15" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M15" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P15" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R15" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15.124000000000001</v>
+      </c>
+      <c r="B16" s="6">
+        <v>29.68</v>
+      </c>
+      <c r="C16" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D16" s="4">
+        <v>638</v>
+      </c>
+      <c r="E16" s="4">
+        <v>638</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G16" s="3">
+        <v>772</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2164</v>
+      </c>
+      <c r="I16" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O16" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P16" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>2033</v>
+      </c>
+      <c r="R16" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16.198</v>
+      </c>
+      <c r="B17" s="6">
+        <v>29.05</v>
+      </c>
+      <c r="C17" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D17" s="4">
+        <v>638</v>
+      </c>
+      <c r="E17" s="4">
+        <v>646</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G17" s="3">
+        <v>772</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2068</v>
+      </c>
+      <c r="I17" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2109</v>
+      </c>
+      <c r="O17" s="4">
+        <v>2114</v>
+      </c>
+      <c r="P17" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R17" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17.271999999999998</v>
+      </c>
+      <c r="B18" s="6">
+        <v>30</v>
+      </c>
+      <c r="C18" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D18" s="4">
+        <v>638</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2183</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G18" s="3">
+        <v>772</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I18" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K18" s="4">
+        <v>2086</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2090</v>
+      </c>
+      <c r="M18" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N18" s="4">
+        <v>2181</v>
+      </c>
+      <c r="O18" s="4">
+        <v>2181</v>
+      </c>
+      <c r="P18" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R18" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18.346</v>
+      </c>
+      <c r="B19" s="6">
+        <v>30</v>
+      </c>
+      <c r="C19" s="7">
+        <v>23.12</v>
+      </c>
+      <c r="D19" s="4">
+        <v>638</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G19" s="3">
+        <v>772</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2124</v>
+      </c>
+      <c r="I19" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J19" s="4">
+        <v>2080</v>
+      </c>
+      <c r="K19" s="4">
+        <v>2102</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M19" s="3">
+        <v>2102</v>
+      </c>
+      <c r="N19" s="4">
+        <v>3404</v>
+      </c>
+      <c r="O19" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P19" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R19" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19.420000000000002</v>
+      </c>
+      <c r="B20" s="6">
+        <v>30.32</v>
+      </c>
+      <c r="C20" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D20" s="4">
+        <v>638</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2183</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G20" s="3">
+        <v>772</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2124</v>
+      </c>
+      <c r="I20" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J20" s="4">
+        <v>2079</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2079</v>
+      </c>
+      <c r="L20" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1530</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1530</v>
+      </c>
+      <c r="O20" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P20" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R20" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20.494</v>
+      </c>
+      <c r="B21" s="6">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D21" s="4">
+        <v>638</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F21" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G21" s="3">
+        <v>772</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2124</v>
+      </c>
+      <c r="I21" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J21" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K21" s="4">
+        <v>2077</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M21" s="3">
+        <v>471</v>
+      </c>
+      <c r="N21" s="4">
+        <v>475</v>
+      </c>
+      <c r="O21" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P21" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>2033</v>
+      </c>
+      <c r="R21" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>21.568000000000001</v>
+      </c>
+      <c r="B22" s="6">
+        <v>30</v>
+      </c>
+      <c r="C22" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D22" s="4">
+        <v>638</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F22" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G22" s="3">
+        <v>772</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2127</v>
+      </c>
+      <c r="I22" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K22" s="4">
+        <v>2086</v>
+      </c>
+      <c r="L22" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M22" s="3">
+        <v>467</v>
+      </c>
+      <c r="N22" s="4">
+        <v>2793</v>
+      </c>
+      <c r="O22" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P22" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>2033</v>
+      </c>
+      <c r="R22" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>22.641999999999999</v>
+      </c>
+      <c r="B23" s="6">
+        <v>30.32</v>
+      </c>
+      <c r="C23" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D23" s="4">
+        <v>638</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F23" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G23" s="3">
+        <v>772</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I23" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2099</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M23" s="3">
+        <v>467</v>
+      </c>
+      <c r="N23" s="4">
+        <v>3394</v>
+      </c>
+      <c r="O23" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P23" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R23" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>23.716000000000001</v>
+      </c>
+      <c r="B24" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C24" s="7">
+        <v>23.31</v>
+      </c>
+      <c r="D24" s="4">
+        <v>638</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2178</v>
+      </c>
+      <c r="F24" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G24" s="3">
+        <v>772</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J24" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K24" s="4">
+        <v>2078</v>
+      </c>
+      <c r="L24" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M24" s="3">
+        <v>467</v>
+      </c>
+      <c r="N24" s="4">
+        <v>480</v>
+      </c>
+      <c r="O24" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P24" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>2035</v>
+      </c>
+      <c r="R24" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>24.79</v>
+      </c>
+      <c r="B25" s="6">
+        <v>30</v>
+      </c>
+      <c r="C25" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D25" s="4">
+        <v>638</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F25" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G25" s="3">
+        <v>772</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I25" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J25" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K25" s="4">
+        <v>2082</v>
+      </c>
+      <c r="L25" s="4">
+        <v>2102</v>
+      </c>
+      <c r="M25" s="3">
+        <v>467</v>
+      </c>
+      <c r="N25" s="4">
+        <v>3143</v>
+      </c>
+      <c r="O25" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P25" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R25" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>25.864000000000001</v>
+      </c>
+      <c r="B26" s="6">
+        <v>30.63</v>
+      </c>
+      <c r="C26" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D26" s="4">
+        <v>638</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2185</v>
+      </c>
+      <c r="F26" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G26" s="3">
+        <v>772</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2124</v>
+      </c>
+      <c r="I26" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J26" s="4">
+        <v>2071</v>
+      </c>
+      <c r="K26" s="4">
+        <v>2083</v>
+      </c>
+      <c r="L26" s="4">
+        <v>2103</v>
+      </c>
+      <c r="M26" s="3">
+        <v>467</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2110</v>
+      </c>
+      <c r="O26" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P26" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R26" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>26.937999999999999</v>
+      </c>
+      <c r="B27" s="6">
+        <v>30.32</v>
+      </c>
+      <c r="C27" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D27" s="4">
+        <v>638</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2181</v>
+      </c>
+      <c r="F27" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G27" s="3">
+        <v>772</v>
+      </c>
+      <c r="H27" s="4">
+        <v>2128</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J27" s="4">
+        <v>522</v>
+      </c>
+      <c r="K27" s="4">
+        <v>524</v>
+      </c>
+      <c r="L27" s="4">
+        <v>2103</v>
+      </c>
+      <c r="M27" s="3">
+        <v>467</v>
+      </c>
+      <c r="N27" s="4">
+        <v>2171</v>
+      </c>
+      <c r="O27" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P27" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R27" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>28.012</v>
+      </c>
+      <c r="B28" s="6">
+        <v>30.32</v>
+      </c>
+      <c r="C28" s="7">
+        <v>23.31</v>
+      </c>
+      <c r="D28" s="4">
+        <v>638</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2182</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G28" s="3">
+        <v>772</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2123</v>
+      </c>
+      <c r="I28" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J28" s="4">
+        <v>518</v>
+      </c>
+      <c r="K28" s="4">
+        <v>3007</v>
+      </c>
+      <c r="L28" s="4">
+        <v>3007</v>
+      </c>
+      <c r="M28" s="3">
+        <v>467</v>
+      </c>
+      <c r="N28" s="4">
+        <v>2100</v>
+      </c>
+      <c r="O28" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P28" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R28" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>29.085999999999999</v>
+      </c>
+      <c r="B29" s="6">
+        <v>30.63</v>
+      </c>
+      <c r="C29" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D29" s="4">
+        <v>638</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2181</v>
+      </c>
+      <c r="F29" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G29" s="3">
+        <v>772</v>
+      </c>
+      <c r="H29" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I29" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J29" s="4">
+        <v>518</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3217</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M29" s="3">
+        <v>467</v>
+      </c>
+      <c r="N29" s="4">
+        <v>2101</v>
+      </c>
+      <c r="O29" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P29" s="6">
+        <v>2031</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>2034</v>
+      </c>
+      <c r="R29" s="7">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>30.16</v>
+      </c>
+      <c r="B30" s="6">
+        <v>30.32</v>
+      </c>
+      <c r="C30" s="7">
+        <v>23.31</v>
+      </c>
+      <c r="D30" s="4">
+        <v>638</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G30" s="3">
+        <v>772</v>
+      </c>
+      <c r="H30" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I30" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J30" s="4">
+        <v>518</v>
+      </c>
+      <c r="K30" s="4">
+        <v>2083</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M30" s="3">
+        <v>467</v>
+      </c>
+      <c r="N30" s="4">
+        <v>2107</v>
+      </c>
+      <c r="O30" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P30" s="6">
+        <v>2026</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>2026</v>
+      </c>
+      <c r="R30" s="7">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>31.234000000000002</v>
+      </c>
+      <c r="B31" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C31" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D31" s="4">
+        <v>638</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2184</v>
+      </c>
+      <c r="F31" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G31" s="3">
+        <v>772</v>
+      </c>
+      <c r="H31" s="4">
+        <v>2123</v>
+      </c>
+      <c r="I31" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J31" s="4">
+        <v>518</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M31" s="3">
+        <v>467</v>
+      </c>
+      <c r="N31" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O31" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P31" s="6">
+        <v>1398</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>1400</v>
+      </c>
+      <c r="R31" s="7">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>32.308</v>
+      </c>
+      <c r="B32" s="6">
+        <v>30.63</v>
+      </c>
+      <c r="C32" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D32" s="4">
+        <v>638</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2178</v>
+      </c>
+      <c r="F32" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G32" s="3">
+        <v>772</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2124</v>
+      </c>
+      <c r="I32" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J32" s="4">
+        <v>518</v>
+      </c>
+      <c r="K32" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L32" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M32" s="3">
+        <v>467</v>
+      </c>
+      <c r="N32" s="4">
+        <v>2109</v>
+      </c>
+      <c r="O32" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P32" s="6">
+        <v>1398</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>2618</v>
+      </c>
+      <c r="R32" s="7">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>33.381999999999998</v>
+      </c>
+      <c r="B33" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C33" s="7">
+        <v>23.31</v>
+      </c>
+      <c r="D33" s="4">
+        <v>638</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2182</v>
+      </c>
+      <c r="F33" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G33" s="3">
+        <v>772</v>
+      </c>
+      <c r="H33" s="4">
+        <v>2126</v>
+      </c>
+      <c r="I33" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J33" s="4">
+        <v>518</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2084</v>
+      </c>
+      <c r="L33" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M33" s="3">
+        <v>467</v>
+      </c>
+      <c r="N33" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O33" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P33" s="6">
+        <v>1398</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>2621</v>
+      </c>
+      <c r="R33" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>34.456000000000003</v>
+      </c>
+      <c r="B34" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C34" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D34" s="4">
+        <v>638</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2181</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G34" s="3">
+        <v>772</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2125</v>
+      </c>
+      <c r="I34" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J34" s="4">
+        <v>518</v>
+      </c>
+      <c r="K34" s="4">
+        <v>2079</v>
+      </c>
+      <c r="L34" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M34" s="3">
+        <v>467</v>
+      </c>
+      <c r="N34" s="4">
+        <v>2105</v>
+      </c>
+      <c r="O34" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P34" s="6">
+        <v>1398</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>1398</v>
+      </c>
+      <c r="R34" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>35.53</v>
+      </c>
+      <c r="B35" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C35" s="7">
+        <v>23.19</v>
+      </c>
+      <c r="D35" s="4">
+        <v>638</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2179</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G35" s="3">
+        <v>772</v>
+      </c>
+      <c r="H35" s="4">
+        <v>2126</v>
+      </c>
+      <c r="I35" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J35" s="4">
+        <v>518</v>
+      </c>
+      <c r="K35" s="4">
+        <v>2085</v>
+      </c>
+      <c r="L35" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M35" s="3">
+        <v>467</v>
+      </c>
+      <c r="N35" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O35" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P35" s="6">
+        <v>1395</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>1406</v>
+      </c>
+      <c r="R35" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>36.603999999999999</v>
+      </c>
+      <c r="B36" s="6">
+        <v>30.63</v>
+      </c>
+      <c r="C36" s="7">
+        <v>23.38</v>
+      </c>
+      <c r="D36" s="4">
+        <v>638</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2185</v>
+      </c>
+      <c r="F36" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G36" s="3">
+        <v>772</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2276</v>
+      </c>
+      <c r="I36" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J36" s="4">
+        <v>518</v>
+      </c>
+      <c r="K36" s="4">
+        <v>2081</v>
+      </c>
+      <c r="L36" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M36" s="3">
+        <v>467</v>
+      </c>
+      <c r="N36" s="4">
+        <v>2108</v>
+      </c>
+      <c r="O36" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P36" s="6">
+        <v>1395</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>2086</v>
+      </c>
+      <c r="R36" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>37.677999999999997</v>
+      </c>
+      <c r="B37" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C37" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D37" s="4">
+        <v>638</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2180</v>
+      </c>
+      <c r="F37" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G37" s="3">
+        <v>772</v>
+      </c>
+      <c r="H37" s="4">
+        <v>3296</v>
+      </c>
+      <c r="I37" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J37" s="4">
+        <v>518</v>
+      </c>
+      <c r="K37" s="4">
+        <v>2082</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M37" s="3">
+        <v>467</v>
+      </c>
+      <c r="N37" s="4">
+        <v>2106</v>
+      </c>
+      <c r="O37" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P37" s="6">
+        <v>1395</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>2087</v>
+      </c>
+      <c r="R37" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>38.752000000000002</v>
+      </c>
+      <c r="B38" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="C38" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="D38" s="4">
+        <v>638</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2179</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3433</v>
+      </c>
+      <c r="G38" s="3">
+        <v>772</v>
+      </c>
+      <c r="H38" s="4">
+        <v>3295</v>
+      </c>
+      <c r="I38" s="5">
+        <v>3312</v>
+      </c>
+      <c r="J38" s="4">
+        <v>518</v>
+      </c>
+      <c r="K38" s="4">
+        <v>2082</v>
+      </c>
+      <c r="L38" s="4">
+        <v>3483</v>
+      </c>
+      <c r="M38" s="3">
+        <v>467</v>
+      </c>
+      <c r="N38" s="4">
+        <v>2112</v>
+      </c>
+      <c r="O38" s="4">
+        <v>3404</v>
+      </c>
+      <c r="P38" s="6">
+        <v>1395</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>2087</v>
+      </c>
+      <c r="R38" s="7">
+        <v>2623</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
@@ -17420,14 +19970,121 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>30.95</v>
+      </c>
+      <c r="B6" s="7">
+        <v>23.25</v>
+      </c>
+      <c r="C6">
+        <v>638</v>
+      </c>
+      <c r="D6">
+        <v>2179</v>
+      </c>
+      <c r="E6">
+        <v>3433</v>
+      </c>
+      <c r="F6" s="3">
+        <v>772</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3295</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3312</v>
+      </c>
+      <c r="I6">
+        <v>518</v>
+      </c>
+      <c r="J6">
+        <v>2082</v>
+      </c>
+      <c r="K6" s="5">
+        <v>3483</v>
+      </c>
+      <c r="L6">
+        <v>467</v>
+      </c>
+      <c r="M6">
+        <v>2112</v>
+      </c>
+      <c r="N6">
+        <v>3404</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1395</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2087</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>2623</v>
+      </c>
+      <c r="S6" s="6">
+        <f>C6-C$4</f>
+        <v>14</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" ref="T6" si="15">D6-D$4</f>
+        <v>-13</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" ref="U6" si="16">E6-E$4</f>
+        <v>-31</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" ref="V6" si="17">F6-F$4</f>
+        <v>24</v>
+      </c>
+      <c r="W6" s="4">
+        <f t="shared" ref="W6" si="18">G6-G$4</f>
+        <v>-34</v>
+      </c>
+      <c r="X6" s="5">
+        <f t="shared" ref="X6" si="19">H6-H$4</f>
+        <v>-66</v>
+      </c>
+      <c r="Y6" s="4">
+        <f t="shared" ref="Y6" si="20">I6-I$4</f>
+        <v>16</v>
+      </c>
+      <c r="Z6" s="4">
+        <f t="shared" ref="Z6" si="21">J6-J$4</f>
+        <v>-11</v>
+      </c>
+      <c r="AA6" s="5">
+        <f t="shared" ref="AA6" si="22">K6-K$4</f>
+        <v>-56</v>
+      </c>
+      <c r="AB6" s="4">
+        <f t="shared" ref="AB6" si="23">L6-L$4</f>
+        <v>16</v>
+      </c>
+      <c r="AC6" s="4">
+        <f t="shared" ref="AC6" si="24">M6-M$4</f>
+        <v>-14</v>
+      </c>
+      <c r="AD6" s="7">
+        <f t="shared" ref="AD6" si="25">N6-N$4</f>
+        <v>-28</v>
+      </c>
+      <c r="AE6" s="6">
+        <f t="shared" ref="AE6" si="26">O6-O$4</f>
+        <v>-5</v>
+      </c>
+      <c r="AF6" s="4">
+        <f t="shared" ref="AF6" si="27">P6-P$4</f>
+        <v>7</v>
+      </c>
+      <c r="AG6" s="7">
+        <f t="shared" ref="AG6" si="28">Q6-Q$4</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="S1:AD1"/>
-    <mergeCell ref="AE1:AG2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="O1:Q2"/>
@@ -17435,6 +20092,12 @@
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
+    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="AE1:AG2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>